<commit_message>
changes to cleaning script
</commit_message>
<xml_diff>
--- a/data/raw/curr_station_rubric.xlsx
+++ b/data/raw/curr_station_rubric.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29721"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29628"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="455" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EDDC200B-DEAA-4B4C-BF83-CA14C0498135}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kylec\Downloads\i379c\bikeshare_analysis\data\raw\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27A357E4-9594-4C27-B435-740BF8C13301}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -127,9 +132,6 @@
     <t>✓</t>
   </si>
   <si>
-    <t>Barton Springs/Bouldin@ Palmer Auditorium</t>
-  </si>
-  <si>
     <t>Barton Springs/Kinney</t>
   </si>
   <si>
@@ -163,18 +165,6 @@
     <t>E 11th/Waller</t>
   </si>
   <si>
-    <t>E 12th/San Jacinto @ State Cap Visitors Garage</t>
-  </si>
-  <si>
-    <t>E 13th/Trinity @ Waterloo Greenway</t>
-  </si>
-  <si>
-    <t>E 21st/Speedway @ PCL</t>
-  </si>
-  <si>
-    <t>E 23rd/San Jacinto @ DKR Stadium</t>
-  </si>
-  <si>
     <t>E 2nd/Congress</t>
   </si>
   <si>
@@ -184,9 +174,6 @@
     <t>E 4th/Chicon</t>
   </si>
   <si>
-    <t>E 5th/Neches @ Downtown Station</t>
-  </si>
-  <si>
     <t>E 5th/Broadway</t>
   </si>
   <si>
@@ -211,12 +198,6 @@
     <t>E 8th/Trinity</t>
   </si>
   <si>
-    <t>Electric Drive @ Pfluger Ped Bridge</t>
-  </si>
-  <si>
-    <t>Guadalupe/West Mall @ University Co-op</t>
-  </si>
-  <si>
     <t>Hollow Creek/Barton Hills</t>
   </si>
   <si>
@@ -229,9 +210,6 @@
     <t>Lakeshore/Pleasant Valley</t>
   </si>
   <si>
-    <t>Nash Hernandez/East @ RBJ South</t>
-  </si>
-  <si>
     <t>One Texas Center</t>
   </si>
   <si>
@@ -250,12 +228,6 @@
     <t>Rosewood/Angelina</t>
   </si>
   <si>
-    <t>S 1st/Riverside @ Long Center</t>
-  </si>
-  <si>
-    <t>South Congress @ Bouldin Creek</t>
-  </si>
-  <si>
     <t>South Congress/Academy</t>
   </si>
   <si>
@@ -271,12 +243,6 @@
     <t>South Congress/Mary</t>
   </si>
   <si>
-    <t>Veterans/Atlanta @ MoPac Ped Bridge</t>
-  </si>
-  <si>
-    <t>W 11th/Congress @ The Texas Capitol</t>
-  </si>
-  <si>
     <t xml:space="preserve">W 16th/San Antonio </t>
   </si>
   <si>
@@ -301,9 +267,6 @@
     <t>W 28th/Rio Grande</t>
   </si>
   <si>
-    <t>W 2nd/Lavaca @ City Hall</t>
-  </si>
-  <si>
     <t>W 3rd/Nueces</t>
   </si>
   <si>
@@ -346,9 +309,6 @@
     <t>30th/Whitis</t>
   </si>
   <si>
-    <t>E 5th/Shady @ Eastside Bus Plaza</t>
-  </si>
-  <si>
     <t xml:space="preserve">E 7th/Pleasant Valley </t>
   </si>
   <si>
@@ -358,20 +318,65 @@
     <t xml:space="preserve">E Cesar Chavez/Pleasant Valley </t>
   </si>
   <si>
-    <t>W 4th/Guadalupe @ Republic Square</t>
-  </si>
-  <si>
     <t>Webberville/Northwestern</t>
   </si>
   <si>
     <t>STATION STATUS - EFFICIENCY</t>
+  </si>
+  <si>
+    <t>Barton Springs/Bouldin@Palmer Auditorium</t>
+  </si>
+  <si>
+    <t>E 12th/San Jacinto@State Cap Visitors Garage</t>
+  </si>
+  <si>
+    <t>E 13th/Trinity@Waterloo Greenway</t>
+  </si>
+  <si>
+    <t>E 21st/Speedway@PCL</t>
+  </si>
+  <si>
+    <t>E 23rd/San Jacinto@DKR Stadium</t>
+  </si>
+  <si>
+    <t>E 5th/Neches@Downtown Station</t>
+  </si>
+  <si>
+    <t>Electric Drive@Pfluger Ped Bridge</t>
+  </si>
+  <si>
+    <t>Guadalupe/West Mall@University Co-op</t>
+  </si>
+  <si>
+    <t>Nash Hernandez/East@RBJ South</t>
+  </si>
+  <si>
+    <t>S 1st/Riverside@Long Center</t>
+  </si>
+  <si>
+    <t>South Congress@Bouldin Creek</t>
+  </si>
+  <si>
+    <t>Veterans/Atlanta@MoPac Ped Bridge</t>
+  </si>
+  <si>
+    <t>W 11th/Congress@The Texas Capitol</t>
+  </si>
+  <si>
+    <t>W 2nd/Lavaca@City Hall</t>
+  </si>
+  <si>
+    <t>W 4th/Guadalupe@Republic Square</t>
+  </si>
+  <si>
+    <t>E 5th/Shady@Eastside Bus Plaza</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -434,6 +439,14 @@
       <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="8">
@@ -567,10 +580,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -651,8 +665,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1045,21 +1061,21 @@
   <dimension ref="A2:S87"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B56" sqref="B56"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="18.28515625" customWidth="1"/>
-    <col min="3" max="3" width="32.140625" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" customWidth="1"/>
+    <col min="2" max="2" width="18.33203125" customWidth="1"/>
+    <col min="3" max="3" width="32.109375" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" customWidth="1"/>
     <col min="5" max="5" width="11" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" customWidth="1"/>
-    <col min="10" max="10" width="17.28515625" customWidth="1"/>
-    <col min="11" max="19" width="18.42578125" customWidth="1"/>
+    <col min="6" max="6" width="12.44140625" customWidth="1"/>
+    <col min="10" max="10" width="17.33203125" customWidth="1"/>
+    <col min="11" max="19" width="18.44140625" customWidth="1"/>
     <col min="20" max="20" width="18" customWidth="1"/>
-    <col min="23" max="23" width="16.85546875" customWidth="1"/>
+    <col min="23" max="23" width="16.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:19" ht="30" customHeight="1">
@@ -1168,11 +1184,11 @@
         <v>11</v>
       </c>
       <c r="G4" s="9">
-        <f>E4/F4</f>
+        <f t="shared" ref="G4:G10" si="0">E4/F4</f>
         <v>231</v>
       </c>
       <c r="H4" s="10">
-        <f>G4/$H$2</f>
+        <f t="shared" ref="H4:H35" si="1">G4/$H$2</f>
         <v>0.64166666666666672</v>
       </c>
       <c r="I4" s="10"/>
@@ -1204,11 +1220,11 @@
         <v>3</v>
       </c>
       <c r="S4" s="5">
-        <f>SUM(J4:R4)</f>
+        <f t="shared" ref="S4:S35" si="2">SUM(J4:R4)</f>
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="15.75">
+    <row r="5" spans="1:19" ht="15.6">
       <c r="A5" s="14">
         <v>39</v>
       </c>
@@ -1228,11 +1244,11 @@
         <v>15</v>
       </c>
       <c r="G5" s="9">
-        <f>E5/F5</f>
+        <f t="shared" si="0"/>
         <v>159.26666666666668</v>
       </c>
       <c r="H5" s="10">
-        <f>G5/$H$2</f>
+        <f t="shared" si="1"/>
         <v>0.44240740740740747</v>
       </c>
       <c r="I5" s="43" t="s">
@@ -1266,7 +1282,7 @@
         <v>3</v>
       </c>
       <c r="S5" s="5">
-        <f>SUM(J5:R5)</f>
+        <f t="shared" si="2"/>
         <v>21</v>
       </c>
     </row>
@@ -1278,7 +1294,7 @@
         <v>45497</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>24</v>
+        <v>88</v>
       </c>
       <c r="D6" s="1">
         <v>9</v>
@@ -1290,11 +1306,11 @@
         <v>15</v>
       </c>
       <c r="G6" s="9">
-        <f>E6/F6</f>
+        <f t="shared" si="0"/>
         <v>228.33333333333334</v>
       </c>
       <c r="H6" s="10">
-        <f>G6/$H$2</f>
+        <f t="shared" si="1"/>
         <v>0.6342592592592593</v>
       </c>
       <c r="I6" s="10"/>
@@ -1326,7 +1342,7 @@
         <v>3</v>
       </c>
       <c r="S6" s="5">
-        <f>SUM(J6:R6)</f>
+        <f t="shared" si="2"/>
         <v>22</v>
       </c>
     </row>
@@ -1338,7 +1354,7 @@
         <v>45610</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D7" s="1">
         <v>9</v>
@@ -1350,11 +1366,11 @@
         <v>11</v>
       </c>
       <c r="G7" s="9">
-        <f>E7/F7</f>
+        <f t="shared" si="0"/>
         <v>180.18181818181819</v>
       </c>
       <c r="H7" s="10">
-        <f>G7/$H$2</f>
+        <f t="shared" si="1"/>
         <v>0.50050505050505056</v>
       </c>
       <c r="I7" s="10"/>
@@ -1386,7 +1402,7 @@
         <v>3</v>
       </c>
       <c r="S7" s="5">
-        <f>SUM(J7:R7)</f>
+        <f t="shared" si="2"/>
         <v>21</v>
       </c>
     </row>
@@ -1398,7 +1414,7 @@
         <v>45610</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D8" s="1">
         <v>9</v>
@@ -1410,11 +1426,11 @@
         <v>11</v>
       </c>
       <c r="G8" s="9">
-        <f>E8/F8</f>
+        <f t="shared" si="0"/>
         <v>246.45454545454547</v>
       </c>
       <c r="H8" s="10">
-        <f>G8/$H$2</f>
+        <f t="shared" si="1"/>
         <v>0.68459595959595965</v>
       </c>
       <c r="I8" s="10"/>
@@ -1446,7 +1462,7 @@
         <v>3</v>
       </c>
       <c r="S8" s="5">
-        <f>SUM(J8:R8)</f>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
     </row>
@@ -1458,7 +1474,7 @@
         <v>45497</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D9" s="1">
         <v>9</v>
@@ -1470,11 +1486,11 @@
         <v>15</v>
       </c>
       <c r="G9" s="9">
-        <f>E9/F9</f>
+        <f t="shared" si="0"/>
         <v>199.8</v>
       </c>
       <c r="H9" s="10">
-        <f>G9/$H$2</f>
+        <f t="shared" si="1"/>
         <v>0.55500000000000005</v>
       </c>
       <c r="I9" s="10"/>
@@ -1506,7 +1522,7 @@
         <v>3</v>
       </c>
       <c r="S9" s="5">
-        <f>SUM(J9:R9)</f>
+        <f t="shared" si="2"/>
         <v>22</v>
       </c>
     </row>
@@ -1518,7 +1534,7 @@
         <v>45610</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D10" s="1">
         <v>1</v>
@@ -1530,11 +1546,11 @@
         <v>11</v>
       </c>
       <c r="G10" s="9">
-        <f>E10/F10</f>
+        <f t="shared" si="0"/>
         <v>190.90909090909091</v>
       </c>
       <c r="H10" s="10">
-        <f>G10/$H$2</f>
+        <f t="shared" si="1"/>
         <v>0.53030303030303028</v>
       </c>
       <c r="I10" s="10"/>
@@ -1566,7 +1582,7 @@
         <v>3</v>
       </c>
       <c r="S10" s="5">
-        <f>SUM(J10:R10)</f>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
     </row>
@@ -1578,7 +1594,7 @@
         <v>45497</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D11" s="1">
         <v>9</v>
@@ -1594,7 +1610,7 @@
         <v>1156</v>
       </c>
       <c r="H11" s="10">
-        <f>G11/$H$2</f>
+        <f t="shared" si="1"/>
         <v>3.2111111111111112</v>
       </c>
       <c r="I11" s="10"/>
@@ -1626,7 +1642,7 @@
         <v>3</v>
       </c>
       <c r="S11" s="5">
-        <f>SUM(J11:R11)</f>
+        <f t="shared" si="2"/>
         <v>25</v>
       </c>
     </row>
@@ -1638,7 +1654,7 @@
         <v>45497</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D12" s="1">
         <v>9</v>
@@ -1650,11 +1666,11 @@
         <v>19</v>
       </c>
       <c r="G12" s="9">
-        <f>E12/F12</f>
+        <f t="shared" ref="G12:G59" si="3">E12/F12</f>
         <v>832.63157894736844</v>
       </c>
       <c r="H12" s="10">
-        <f>G12/$H$2</f>
+        <f t="shared" si="1"/>
         <v>2.3128654970760234</v>
       </c>
       <c r="I12" s="10"/>
@@ -1686,7 +1702,7 @@
         <v>3</v>
       </c>
       <c r="S12" s="5">
-        <f>SUM(J12:R12)</f>
+        <f t="shared" si="2"/>
         <v>23</v>
       </c>
     </row>
@@ -1698,7 +1714,7 @@
         <v>45497</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D13" s="1">
         <v>9</v>
@@ -1710,11 +1726,11 @@
         <v>15</v>
       </c>
       <c r="G13" s="9">
-        <f>E13/F13</f>
+        <f t="shared" si="3"/>
         <v>95.666666666666671</v>
       </c>
       <c r="H13" s="10">
-        <f>G13/$H$2</f>
+        <f t="shared" si="1"/>
         <v>0.26574074074074078</v>
       </c>
       <c r="I13" s="10"/>
@@ -1746,7 +1762,7 @@
         <v>3</v>
       </c>
       <c r="S13" s="5">
-        <f>SUM(J13:R13)</f>
+        <f t="shared" si="2"/>
         <v>19</v>
       </c>
     </row>
@@ -1758,7 +1774,7 @@
         <v>45499</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D14" s="1">
         <v>1</v>
@@ -1770,11 +1786,11 @@
         <v>11</v>
       </c>
       <c r="G14" s="9">
-        <f>E14/F14</f>
+        <f t="shared" si="3"/>
         <v>77.545454545454547</v>
       </c>
       <c r="H14" s="10">
-        <f>G14/$H$2</f>
+        <f t="shared" si="1"/>
         <v>0.2154040404040404</v>
       </c>
       <c r="I14" s="10"/>
@@ -1806,7 +1822,7 @@
         <v>3</v>
       </c>
       <c r="S14" s="5">
-        <f>SUM(J14:R14)</f>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
     </row>
@@ -1818,7 +1834,7 @@
         <v>45610</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D15" s="1">
         <v>9</v>
@@ -1830,11 +1846,11 @@
         <v>11</v>
       </c>
       <c r="G15" s="9">
-        <f>E15/F15</f>
+        <f t="shared" si="3"/>
         <v>58.636363636363633</v>
       </c>
       <c r="H15" s="10">
-        <f>G15/$H$2</f>
+        <f t="shared" si="1"/>
         <v>0.16287878787878787</v>
       </c>
       <c r="I15" s="10"/>
@@ -1866,7 +1882,7 @@
         <v>3</v>
       </c>
       <c r="S15" s="5">
-        <f>SUM(J15:R15)</f>
+        <f t="shared" si="2"/>
         <v>21</v>
       </c>
     </row>
@@ -1878,7 +1894,7 @@
         <v>45610</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D16" s="1">
         <v>1</v>
@@ -1890,11 +1906,11 @@
         <v>11</v>
       </c>
       <c r="G16" s="9">
-        <f>E16/F16</f>
+        <f t="shared" si="3"/>
         <v>174.90909090909091</v>
       </c>
       <c r="H16" s="10">
-        <f>G16/$H$2</f>
+        <f t="shared" si="1"/>
         <v>0.48585858585858588</v>
       </c>
       <c r="I16" s="10"/>
@@ -1926,7 +1942,7 @@
         <v>3</v>
       </c>
       <c r="S16" s="5">
-        <f>SUM(J16:R16)</f>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
     </row>
@@ -1938,7 +1954,7 @@
         <v>45610</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D17" s="1">
         <v>1</v>
@@ -1950,11 +1966,11 @@
         <v>11</v>
       </c>
       <c r="G17" s="9">
-        <f>E17/F17</f>
+        <f t="shared" si="3"/>
         <v>56.272727272727273</v>
       </c>
       <c r="H17" s="10">
-        <f>G17/$H$2</f>
+        <f t="shared" si="1"/>
         <v>0.15631313131313132</v>
       </c>
       <c r="I17" s="10"/>
@@ -1986,7 +2002,7 @@
         <v>3</v>
       </c>
       <c r="S17" s="5">
-        <f>SUM(J17:R17)</f>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
     </row>
@@ -1998,7 +2014,7 @@
         <v>45497</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>36</v>
+        <v>89</v>
       </c>
       <c r="D18" s="1">
         <v>9</v>
@@ -2010,11 +2026,11 @@
         <v>11</v>
       </c>
       <c r="G18" s="9">
-        <f>E18/F18</f>
+        <f t="shared" si="3"/>
         <v>60</v>
       </c>
       <c r="H18" s="10">
-        <f>G18/$H$2</f>
+        <f t="shared" si="1"/>
         <v>0.16666666666666666</v>
       </c>
       <c r="I18" s="10"/>
@@ -2046,7 +2062,7 @@
         <v>3</v>
       </c>
       <c r="S18" s="5">
-        <f>SUM(J18:R18)</f>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
     </row>
@@ -2058,7 +2074,7 @@
         <v>45497</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>37</v>
+        <v>90</v>
       </c>
       <c r="D19" s="1">
         <v>9</v>
@@ -2070,11 +2086,11 @@
         <v>11</v>
       </c>
       <c r="G19" s="9">
-        <f>E19/F19</f>
+        <f t="shared" si="3"/>
         <v>103.45454545454545</v>
       </c>
       <c r="H19" s="10">
-        <f>G19/$H$2</f>
+        <f t="shared" si="1"/>
         <v>0.28737373737373739</v>
       </c>
       <c r="I19" s="10"/>
@@ -2106,7 +2122,7 @@
         <v>3</v>
       </c>
       <c r="S19" s="5">
-        <f>SUM(J19:R19)</f>
+        <f t="shared" si="2"/>
         <v>21</v>
       </c>
     </row>
@@ -2118,7 +2134,7 @@
         <v>45610</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>38</v>
+        <v>91</v>
       </c>
       <c r="D20" s="1">
         <v>9</v>
@@ -2130,11 +2146,11 @@
         <v>17</v>
       </c>
       <c r="G20" s="9">
-        <f>E20/F20</f>
+        <f t="shared" si="3"/>
         <v>1788.3529411764705</v>
       </c>
       <c r="H20" s="10">
-        <f>G20/$H$2</f>
+        <f t="shared" si="1"/>
         <v>4.9676470588235295</v>
       </c>
       <c r="I20" s="10"/>
@@ -2166,7 +2182,7 @@
         <v>3</v>
       </c>
       <c r="S20" s="5">
-        <f>SUM(J20:R20)</f>
+        <f t="shared" si="2"/>
         <v>25</v>
       </c>
     </row>
@@ -2178,7 +2194,7 @@
         <v>45610</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>39</v>
+        <v>92</v>
       </c>
       <c r="D21" s="1">
         <v>9</v>
@@ -2190,11 +2206,11 @@
         <v>23</v>
       </c>
       <c r="G21" s="9">
-        <f>E21/F21</f>
+        <f t="shared" si="3"/>
         <v>295.78260869565219</v>
       </c>
       <c r="H21" s="10">
-        <f>G21/$H$2</f>
+        <f t="shared" si="1"/>
         <v>0.82161835748792278</v>
       </c>
       <c r="I21" s="10"/>
@@ -2226,7 +2242,7 @@
         <v>3</v>
       </c>
       <c r="S21" s="5">
-        <f>SUM(J21:R21)</f>
+        <f t="shared" si="2"/>
         <v>24</v>
       </c>
     </row>
@@ -2238,7 +2254,7 @@
         <v>45498</v>
       </c>
       <c r="C22" s="15" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="D22" s="1">
         <v>9</v>
@@ -2250,11 +2266,11 @@
         <v>15</v>
       </c>
       <c r="G22" s="9">
-        <f>E22/F22</f>
+        <f t="shared" si="3"/>
         <v>288.13333333333333</v>
       </c>
       <c r="H22" s="10">
-        <f>G22/$H$2</f>
+        <f t="shared" si="1"/>
         <v>0.8003703703703704</v>
       </c>
       <c r="I22" s="10"/>
@@ -2286,7 +2302,7 @@
         <v>3</v>
       </c>
       <c r="S22" s="5">
-        <f>SUM(J22:R22)</f>
+        <f t="shared" si="2"/>
         <v>21</v>
       </c>
     </row>
@@ -2298,7 +2314,7 @@
         <v>45610</v>
       </c>
       <c r="C23" s="15" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="D23" s="1">
         <v>3</v>
@@ -2310,11 +2326,11 @@
         <v>11</v>
       </c>
       <c r="G23" s="9">
-        <f>E23/F23</f>
+        <f t="shared" si="3"/>
         <v>117.27272727272727</v>
       </c>
       <c r="H23" s="10">
-        <f>G23/$H$2</f>
+        <f t="shared" si="1"/>
         <v>0.32575757575757575</v>
       </c>
       <c r="I23" s="10"/>
@@ -2346,7 +2362,7 @@
         <v>3</v>
       </c>
       <c r="S23" s="5">
-        <f>SUM(J23:R23)</f>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
     </row>
@@ -2358,7 +2374,7 @@
         <v>45503</v>
       </c>
       <c r="C24" s="15" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="D24" s="1">
         <v>3</v>
@@ -2370,11 +2386,11 @@
         <v>19</v>
       </c>
       <c r="G24" s="9">
-        <f>E24/F24</f>
+        <f t="shared" si="3"/>
         <v>94.05263157894737</v>
       </c>
       <c r="H24" s="10">
-        <f>G24/$H$2</f>
+        <f t="shared" si="1"/>
         <v>0.26125730994152047</v>
       </c>
       <c r="I24" s="10"/>
@@ -2406,7 +2422,7 @@
         <v>3</v>
       </c>
       <c r="S24" s="5">
-        <f>SUM(J24:R24)</f>
+        <f t="shared" si="2"/>
         <v>19</v>
       </c>
     </row>
@@ -2418,7 +2434,7 @@
         <v>45504</v>
       </c>
       <c r="C25" s="15" t="s">
-        <v>43</v>
+        <v>93</v>
       </c>
       <c r="D25" s="1">
         <v>9</v>
@@ -2430,11 +2446,11 @@
         <v>15</v>
       </c>
       <c r="G25" s="9">
-        <f>E25/F25</f>
+        <f t="shared" si="3"/>
         <v>277.39999999999998</v>
       </c>
       <c r="H25" s="10">
-        <f>G25/$H$2</f>
+        <f t="shared" si="1"/>
         <v>0.77055555555555544</v>
       </c>
       <c r="I25" s="10"/>
@@ -2466,7 +2482,7 @@
         <v>3</v>
       </c>
       <c r="S25" s="5">
-        <f>SUM(J25:R25)</f>
+        <f t="shared" si="2"/>
         <v>21</v>
       </c>
     </row>
@@ -2478,7 +2494,7 @@
         <v>45505</v>
       </c>
       <c r="C26" s="15" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="D26" s="1">
         <v>3</v>
@@ -2490,11 +2506,11 @@
         <v>15</v>
       </c>
       <c r="G26" s="9">
-        <f>E26/F26</f>
+        <f t="shared" si="3"/>
         <v>156.93333333333334</v>
       </c>
       <c r="H26" s="10">
-        <f>G26/$H$2</f>
+        <f t="shared" si="1"/>
         <v>0.43592592592592594</v>
       </c>
       <c r="I26" s="10"/>
@@ -2526,7 +2542,7 @@
         <v>3</v>
       </c>
       <c r="S26" s="5">
-        <f>SUM(J26:R26)</f>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
     </row>
@@ -2538,7 +2554,7 @@
         <v>45499</v>
       </c>
       <c r="C27" s="15" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D27" s="1">
         <v>3</v>
@@ -2550,11 +2566,11 @@
         <v>11</v>
       </c>
       <c r="G27" s="9">
-        <f>E27/F27</f>
+        <f t="shared" si="3"/>
         <v>146.72727272727272</v>
       </c>
       <c r="H27" s="10">
-        <f>G27/$H$2</f>
+        <f t="shared" si="1"/>
         <v>0.40757575757575754</v>
       </c>
       <c r="I27" s="10"/>
@@ -2586,7 +2602,7 @@
         <v>3</v>
       </c>
       <c r="S27" s="5">
-        <f>SUM(J27:R27)</f>
+        <f t="shared" si="2"/>
         <v>19</v>
       </c>
     </row>
@@ -2598,7 +2614,7 @@
         <v>45497</v>
       </c>
       <c r="C28" s="15" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="D28" s="1">
         <v>3</v>
@@ -2610,11 +2626,11 @@
         <v>11</v>
       </c>
       <c r="G28" s="9">
-        <f>E28/F28</f>
+        <f t="shared" si="3"/>
         <v>121.63636363636364</v>
       </c>
       <c r="H28" s="10">
-        <f>G28/$H$2</f>
+        <f t="shared" si="1"/>
         <v>0.33787878787878789</v>
       </c>
       <c r="I28" s="10"/>
@@ -2646,7 +2662,7 @@
         <v>3</v>
       </c>
       <c r="S28" s="5">
-        <f>SUM(J28:R28)</f>
+        <f t="shared" si="2"/>
         <v>19</v>
       </c>
     </row>
@@ -2658,7 +2674,7 @@
         <v>45497</v>
       </c>
       <c r="C29" s="15" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D29" s="1">
         <v>3</v>
@@ -2670,11 +2686,11 @@
         <v>11</v>
       </c>
       <c r="G29" s="9">
-        <f>E29/F29</f>
+        <f t="shared" si="3"/>
         <v>390.81818181818181</v>
       </c>
       <c r="H29" s="10">
-        <f>G29/$H$2</f>
+        <f t="shared" si="1"/>
         <v>1.0856060606060607</v>
       </c>
       <c r="I29" s="10"/>
@@ -2706,7 +2722,7 @@
         <v>3</v>
       </c>
       <c r="S29" s="5">
-        <f>SUM(J29:R29)</f>
+        <f t="shared" si="2"/>
         <v>22</v>
       </c>
     </row>
@@ -2718,7 +2734,7 @@
         <v>45505</v>
       </c>
       <c r="C30" s="15" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D30" s="1">
         <v>3</v>
@@ -2730,11 +2746,11 @@
         <v>11</v>
       </c>
       <c r="G30" s="9">
-        <f>E30/F30</f>
+        <f t="shared" si="3"/>
         <v>235.27272727272728</v>
       </c>
       <c r="H30" s="10">
-        <f>G30/$H$2</f>
+        <f t="shared" si="1"/>
         <v>0.65353535353535352</v>
       </c>
       <c r="I30" s="10"/>
@@ -2766,7 +2782,7 @@
         <v>3</v>
       </c>
       <c r="S30" s="5">
-        <f>SUM(J30:R30)</f>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
     </row>
@@ -2778,7 +2794,7 @@
         <v>45497</v>
       </c>
       <c r="C31" s="15" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="D31" s="1">
         <v>9</v>
@@ -2790,11 +2806,11 @@
         <v>7</v>
       </c>
       <c r="G31" s="9">
-        <f>E31/F31</f>
+        <f t="shared" si="3"/>
         <v>143.42857142857142</v>
       </c>
       <c r="H31" s="10">
-        <f>G31/$H$2</f>
+        <f t="shared" si="1"/>
         <v>0.39841269841269839</v>
       </c>
       <c r="I31" s="10"/>
@@ -2826,7 +2842,7 @@
         <v>3</v>
       </c>
       <c r="S31" s="5">
-        <f>SUM(J31:R31)</f>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
     </row>
@@ -2838,7 +2854,7 @@
         <v>45497</v>
       </c>
       <c r="C32" s="15" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="D32" s="1">
         <v>9</v>
@@ -2850,11 +2866,11 @@
         <v>11</v>
       </c>
       <c r="G32" s="9">
-        <f>E32/F32</f>
+        <f t="shared" si="3"/>
         <v>135.90909090909091</v>
       </c>
       <c r="H32" s="10">
-        <f>G32/$H$2</f>
+        <f t="shared" si="1"/>
         <v>0.37752525252525254</v>
       </c>
       <c r="I32" s="10"/>
@@ -2886,7 +2902,7 @@
         <v>3</v>
       </c>
       <c r="S32" s="5">
-        <f>SUM(J32:R32)</f>
+        <f t="shared" si="2"/>
         <v>19</v>
       </c>
     </row>
@@ -2898,7 +2914,7 @@
         <v>45610</v>
       </c>
       <c r="C33" s="15" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D33" s="1">
         <v>9</v>
@@ -2910,11 +2926,11 @@
         <v>15</v>
       </c>
       <c r="G33" s="9">
-        <f>E33/F33</f>
+        <f t="shared" si="3"/>
         <v>69.8</v>
       </c>
       <c r="H33" s="10">
-        <f>G33/$H$2</f>
+        <f t="shared" si="1"/>
         <v>0.19388888888888889</v>
       </c>
       <c r="I33" s="10"/>
@@ -2946,7 +2962,7 @@
         <v>3</v>
       </c>
       <c r="S33" s="5">
-        <f>SUM(J33:R33)</f>
+        <f t="shared" si="2"/>
         <v>19</v>
       </c>
     </row>
@@ -2958,7 +2974,7 @@
         <v>45497</v>
       </c>
       <c r="C34" s="15" t="s">
-        <v>52</v>
+        <v>94</v>
       </c>
       <c r="D34" s="1">
         <v>9</v>
@@ -2970,11 +2986,11 @@
         <v>19</v>
       </c>
       <c r="G34" s="9">
-        <f>E34/F34</f>
+        <f t="shared" si="3"/>
         <v>286.78947368421052</v>
       </c>
       <c r="H34" s="10">
-        <f>G34/$H$2</f>
+        <f t="shared" si="1"/>
         <v>0.79663742690058481</v>
       </c>
       <c r="I34" s="10"/>
@@ -3006,7 +3022,7 @@
         <v>3</v>
       </c>
       <c r="S34" s="5">
-        <f>SUM(J34:R34)</f>
+        <f t="shared" si="2"/>
         <v>23</v>
       </c>
     </row>
@@ -3018,7 +3034,7 @@
         <v>45497</v>
       </c>
       <c r="C35" s="15" t="s">
-        <v>53</v>
+        <v>95</v>
       </c>
       <c r="D35" s="1">
         <v>9</v>
@@ -3030,11 +3046,11 @@
         <v>15</v>
       </c>
       <c r="G35" s="9">
-        <f>E35/F35</f>
+        <f t="shared" si="3"/>
         <v>832.5333333333333</v>
       </c>
       <c r="H35" s="10">
-        <f>G35/$H$2</f>
+        <f t="shared" si="1"/>
         <v>2.3125925925925923</v>
       </c>
       <c r="I35" s="10"/>
@@ -3066,7 +3082,7 @@
         <v>3</v>
       </c>
       <c r="S35" s="5">
-        <f>SUM(J35:R35)</f>
+        <f t="shared" si="2"/>
         <v>25</v>
       </c>
     </row>
@@ -3078,7 +3094,7 @@
         <v>45506</v>
       </c>
       <c r="C36" s="15" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="D36" s="1">
         <v>5</v>
@@ -3090,11 +3106,11 @@
         <v>11</v>
       </c>
       <c r="G36" s="9">
-        <f>E36/F36</f>
+        <f t="shared" si="3"/>
         <v>199.09090909090909</v>
       </c>
       <c r="H36" s="10">
-        <f>G36/$H$2</f>
+        <f t="shared" ref="H36:H67" si="4">G36/$H$2</f>
         <v>0.55303030303030298</v>
       </c>
       <c r="I36" s="10"/>
@@ -3126,7 +3142,7 @@
         <v>2</v>
       </c>
       <c r="S36" s="5">
-        <f>SUM(J36:R36)</f>
+        <f t="shared" ref="S36:S67" si="5">SUM(J36:R36)</f>
         <v>16</v>
       </c>
     </row>
@@ -3138,7 +3154,7 @@
         <v>45610</v>
       </c>
       <c r="C37" s="15" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="D37" s="1">
         <v>10</v>
@@ -3150,11 +3166,11 @@
         <v>11</v>
       </c>
       <c r="G37" s="9">
-        <f>E37/F37</f>
+        <f t="shared" si="3"/>
         <v>267</v>
       </c>
       <c r="H37" s="10">
-        <f>G37/$H$2</f>
+        <f t="shared" si="4"/>
         <v>0.7416666666666667</v>
       </c>
       <c r="I37" s="10"/>
@@ -3186,7 +3202,7 @@
         <v>3</v>
       </c>
       <c r="S37" s="5">
-        <f>SUM(J37:R37)</f>
+        <f t="shared" si="5"/>
         <v>22</v>
       </c>
     </row>
@@ -3198,7 +3214,7 @@
         <v>45610</v>
       </c>
       <c r="C38" s="15" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="D38" s="1">
         <v>3</v>
@@ -3210,11 +3226,11 @@
         <v>11</v>
       </c>
       <c r="G38" s="9">
-        <f>E38/F38</f>
+        <f t="shared" si="3"/>
         <v>351.36363636363637</v>
       </c>
       <c r="H38" s="10">
-        <f>G38/$H$2</f>
+        <f t="shared" si="4"/>
         <v>0.97601010101010099</v>
       </c>
       <c r="I38" s="10"/>
@@ -3246,7 +3262,7 @@
         <v>1</v>
       </c>
       <c r="S38" s="5">
-        <f>SUM(J38:R38)</f>
+        <f t="shared" si="5"/>
         <v>18</v>
       </c>
     </row>
@@ -3258,7 +3274,7 @@
         <v>45503</v>
       </c>
       <c r="C39" s="15" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="D39" s="1">
         <v>3</v>
@@ -3270,11 +3286,11 @@
         <v>15</v>
       </c>
       <c r="G39" s="9">
-        <f>E39/F39</f>
+        <f t="shared" si="3"/>
         <v>304.86666666666667</v>
       </c>
       <c r="H39" s="10">
-        <f>G39/$H$2</f>
+        <f t="shared" si="4"/>
         <v>0.84685185185185186</v>
       </c>
       <c r="I39" s="10"/>
@@ -3306,7 +3322,7 @@
         <v>1</v>
       </c>
       <c r="S39" s="5">
-        <f>SUM(J39:R39)</f>
+        <f t="shared" si="5"/>
         <v>19</v>
       </c>
     </row>
@@ -3318,7 +3334,7 @@
         <v>45505</v>
       </c>
       <c r="C40" s="15" t="s">
-        <v>58</v>
+        <v>96</v>
       </c>
       <c r="D40" s="1">
         <v>3</v>
@@ -3330,11 +3346,11 @@
         <v>11</v>
       </c>
       <c r="G40" s="9">
-        <f>E40/F40</f>
+        <f t="shared" si="3"/>
         <v>387.36363636363637</v>
       </c>
       <c r="H40" s="10">
-        <f>G40/$H$2</f>
+        <f t="shared" si="4"/>
         <v>1.0760101010101011</v>
       </c>
       <c r="I40" s="10"/>
@@ -3366,7 +3382,7 @@
         <v>2</v>
       </c>
       <c r="S40" s="5">
-        <f>SUM(J40:R40)</f>
+        <f t="shared" si="5"/>
         <v>23</v>
       </c>
     </row>
@@ -3378,7 +3394,7 @@
         <v>45497</v>
       </c>
       <c r="C41" s="15" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="D41" s="1">
         <v>9</v>
@@ -3390,11 +3406,11 @@
         <v>15</v>
       </c>
       <c r="G41" s="9">
-        <f>E41/F41</f>
+        <f t="shared" si="3"/>
         <v>68.2</v>
       </c>
       <c r="H41" s="10">
-        <f>G41/$H$2</f>
+        <f t="shared" si="4"/>
         <v>0.18944444444444444</v>
       </c>
       <c r="I41" s="10"/>
@@ -3426,7 +3442,7 @@
         <v>3</v>
       </c>
       <c r="S41" s="5">
-        <f>SUM(J41:R41)</f>
+        <f t="shared" si="5"/>
         <v>17</v>
       </c>
     </row>
@@ -3438,7 +3454,7 @@
         <v>45499</v>
       </c>
       <c r="C42" s="15" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D42" s="1">
         <v>3</v>
@@ -3450,11 +3466,11 @@
         <v>15</v>
       </c>
       <c r="G42" s="9">
-        <f>E42/F42</f>
+        <f t="shared" si="3"/>
         <v>352.93333333333334</v>
       </c>
       <c r="H42" s="10">
-        <f>G42/$H$2</f>
+        <f t="shared" si="4"/>
         <v>0.98037037037037034</v>
       </c>
       <c r="I42" s="10"/>
@@ -3486,7 +3502,7 @@
         <v>3</v>
       </c>
       <c r="S42" s="5">
-        <f>SUM(J42:R42)</f>
+        <f t="shared" si="5"/>
         <v>21</v>
       </c>
     </row>
@@ -3498,7 +3514,7 @@
         <v>45497</v>
       </c>
       <c r="C43" s="15" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="D43" s="1">
         <v>9</v>
@@ -3510,11 +3526,11 @@
         <v>19</v>
       </c>
       <c r="G43" s="9">
-        <f>E43/F43</f>
+        <f t="shared" si="3"/>
         <v>543.52631578947364</v>
       </c>
       <c r="H43" s="10">
-        <f>G43/$H$2</f>
+        <f t="shared" si="4"/>
         <v>1.5097953216374267</v>
       </c>
       <c r="I43" s="10"/>
@@ -3546,7 +3562,7 @@
         <v>2</v>
       </c>
       <c r="S43" s="5">
-        <f>SUM(J43:R43)</f>
+        <f t="shared" si="5"/>
         <v>24</v>
       </c>
     </row>
@@ -3558,7 +3574,7 @@
         <v>45497</v>
       </c>
       <c r="C44" s="15" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="D44" s="1">
         <v>9</v>
@@ -3570,11 +3586,11 @@
         <v>11</v>
       </c>
       <c r="G44" s="9">
-        <f>E44/F44</f>
+        <f t="shared" si="3"/>
         <v>296.36363636363637</v>
       </c>
       <c r="H44" s="10">
-        <f>G44/$H$2</f>
+        <f t="shared" si="4"/>
         <v>0.82323232323232332</v>
       </c>
       <c r="I44" s="10"/>
@@ -3606,7 +3622,7 @@
         <v>3</v>
       </c>
       <c r="S44" s="5">
-        <f>SUM(J44:R44)</f>
+        <f t="shared" si="5"/>
         <v>21</v>
       </c>
     </row>
@@ -3618,7 +3634,7 @@
         <v>45497</v>
       </c>
       <c r="C45" s="15" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="D45" s="1">
         <v>9</v>
@@ -3630,11 +3646,11 @@
         <v>19</v>
       </c>
       <c r="G45" s="9">
-        <f>E45/F45</f>
+        <f t="shared" si="3"/>
         <v>393.68421052631578</v>
       </c>
       <c r="H45" s="10">
-        <f>G45/$H$2</f>
+        <f t="shared" si="4"/>
         <v>1.0935672514619883</v>
       </c>
       <c r="I45" s="10"/>
@@ -3666,7 +3682,7 @@
         <v>3</v>
       </c>
       <c r="S45" s="5">
-        <f>SUM(J45:R45)</f>
+        <f t="shared" si="5"/>
         <v>25</v>
       </c>
     </row>
@@ -3678,7 +3694,7 @@
         <v>45499</v>
       </c>
       <c r="C46" s="15" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="D46" s="1">
         <v>1</v>
@@ -3690,11 +3706,11 @@
         <v>11</v>
       </c>
       <c r="G46" s="9">
-        <f>E46/F46</f>
+        <f t="shared" si="3"/>
         <v>72.818181818181813</v>
       </c>
       <c r="H46" s="10">
-        <f>G46/$H$2</f>
+        <f t="shared" si="4"/>
         <v>0.20227272727272727</v>
       </c>
       <c r="I46" s="10"/>
@@ -3726,7 +3742,7 @@
         <v>2</v>
       </c>
       <c r="S46" s="5">
-        <f>SUM(J46:R46)</f>
+        <f t="shared" si="5"/>
         <v>18</v>
       </c>
     </row>
@@ -3738,7 +3754,7 @@
         <v>45497</v>
       </c>
       <c r="C47" s="15" t="s">
-        <v>65</v>
+        <v>97</v>
       </c>
       <c r="D47" s="1">
         <v>9</v>
@@ -3750,11 +3766,11 @@
         <v>15</v>
       </c>
       <c r="G47" s="9">
-        <f>E47/F47</f>
+        <f t="shared" si="3"/>
         <v>196.46666666666667</v>
       </c>
       <c r="H47" s="10">
-        <f>G47/$H$2</f>
+        <f t="shared" si="4"/>
         <v>0.54574074074074075</v>
       </c>
       <c r="I47" s="10"/>
@@ -3786,7 +3802,7 @@
         <v>3</v>
       </c>
       <c r="S47" s="5">
-        <f>SUM(J47:R47)</f>
+        <f t="shared" si="5"/>
         <v>22</v>
       </c>
     </row>
@@ -3798,7 +3814,7 @@
         <v>45502</v>
       </c>
       <c r="C48" s="15" t="s">
-        <v>66</v>
+        <v>98</v>
       </c>
       <c r="D48" s="1">
         <v>9</v>
@@ -3810,11 +3826,11 @@
         <v>15</v>
       </c>
       <c r="G48" s="9">
-        <f>E48/F48</f>
+        <f t="shared" si="3"/>
         <v>148.46666666666667</v>
       </c>
       <c r="H48" s="10">
-        <f>G48/$H$2</f>
+        <f t="shared" si="4"/>
         <v>0.41240740740740739</v>
       </c>
       <c r="I48" s="10"/>
@@ -3846,7 +3862,7 @@
         <v>3</v>
       </c>
       <c r="S48" s="5">
-        <f>SUM(J48:R48)</f>
+        <f t="shared" si="5"/>
         <v>20</v>
       </c>
     </row>
@@ -3858,7 +3874,7 @@
         <v>45610</v>
       </c>
       <c r="C49" s="15" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="D49" s="1">
         <v>9</v>
@@ -3870,11 +3886,11 @@
         <v>11</v>
       </c>
       <c r="G49" s="9">
-        <f>E49/F49</f>
+        <f t="shared" si="3"/>
         <v>143.27272727272728</v>
       </c>
       <c r="H49" s="10">
-        <f>G49/$H$2</f>
+        <f t="shared" si="4"/>
         <v>0.39797979797979799</v>
       </c>
       <c r="I49" s="10"/>
@@ -3906,7 +3922,7 @@
         <v>3</v>
       </c>
       <c r="S49" s="5">
-        <f>SUM(J49:R49)</f>
+        <f t="shared" si="5"/>
         <v>19</v>
       </c>
     </row>
@@ -3918,7 +3934,7 @@
         <v>45498</v>
       </c>
       <c r="C50" s="15" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="D50" s="1">
         <v>9</v>
@@ -3930,11 +3946,11 @@
         <v>11</v>
       </c>
       <c r="G50" s="9">
-        <f>E50/F50</f>
+        <f t="shared" si="3"/>
         <v>247.90909090909091</v>
       </c>
       <c r="H50" s="10">
-        <f>G50/$H$2</f>
+        <f t="shared" si="4"/>
         <v>0.6886363636363636</v>
       </c>
       <c r="I50" s="10"/>
@@ -3966,7 +3982,7 @@
         <v>3</v>
       </c>
       <c r="S50" s="5">
-        <f>SUM(J50:R50)</f>
+        <f t="shared" si="5"/>
         <v>19</v>
       </c>
     </row>
@@ -3978,7 +3994,7 @@
         <v>45502</v>
       </c>
       <c r="C51" s="15" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="D51" s="1">
         <v>9</v>
@@ -3990,11 +4006,11 @@
         <v>11</v>
       </c>
       <c r="G51" s="9">
-        <f>E51/F51</f>
+        <f t="shared" si="3"/>
         <v>128.27272727272728</v>
       </c>
       <c r="H51" s="10">
-        <f>G51/$H$2</f>
+        <f t="shared" si="4"/>
         <v>0.35631313131313136</v>
       </c>
       <c r="I51" s="10"/>
@@ -4026,7 +4042,7 @@
         <v>3</v>
       </c>
       <c r="S51" s="5">
-        <f>SUM(J51:R51)</f>
+        <f t="shared" si="5"/>
         <v>19</v>
       </c>
     </row>
@@ -4038,7 +4054,7 @@
         <v>45506</v>
       </c>
       <c r="C52" s="15" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="D52" s="1">
         <v>9</v>
@@ -4050,11 +4066,11 @@
         <v>7</v>
       </c>
       <c r="G52" s="9">
-        <f>E52/F52</f>
+        <f t="shared" si="3"/>
         <v>161.42857142857142</v>
       </c>
       <c r="H52" s="10">
-        <f>G52/$H$2</f>
+        <f t="shared" si="4"/>
         <v>0.44841269841269837</v>
       </c>
       <c r="I52" s="10"/>
@@ -4086,7 +4102,7 @@
         <v>3</v>
       </c>
       <c r="S52" s="5">
-        <f>SUM(J52:R52)</f>
+        <f t="shared" si="5"/>
         <v>19</v>
       </c>
     </row>
@@ -4098,7 +4114,7 @@
         <v>45497</v>
       </c>
       <c r="C53" s="15" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="D53" s="1">
         <v>9</v>
@@ -4110,11 +4126,11 @@
         <v>11</v>
       </c>
       <c r="G53" s="9">
-        <f>E53/F53</f>
+        <f t="shared" si="3"/>
         <v>192.72727272727272</v>
       </c>
       <c r="H53" s="10">
-        <f>G53/$H$2</f>
+        <f t="shared" si="4"/>
         <v>0.53535353535353536</v>
       </c>
       <c r="I53" s="10"/>
@@ -4146,7 +4162,7 @@
         <v>2</v>
       </c>
       <c r="S53" s="5">
-        <f>SUM(J53:R53)</f>
+        <f t="shared" si="5"/>
         <v>19</v>
       </c>
     </row>
@@ -4157,8 +4173,8 @@
       <c r="B54" s="19">
         <v>45497</v>
       </c>
-      <c r="C54" s="15" t="s">
-        <v>72</v>
+      <c r="C54" s="46" t="s">
+        <v>99</v>
       </c>
       <c r="D54" s="1">
         <v>9</v>
@@ -4170,11 +4186,11 @@
         <v>19</v>
       </c>
       <c r="G54" s="9">
-        <f>E54/F54</f>
+        <f t="shared" si="3"/>
         <v>186.42105263157896</v>
       </c>
       <c r="H54" s="10">
-        <f>G54/$H$2</f>
+        <f t="shared" si="4"/>
         <v>0.51783625730994154</v>
       </c>
       <c r="I54" s="10"/>
@@ -4206,7 +4222,7 @@
         <v>3</v>
       </c>
       <c r="S54" s="5">
-        <f>SUM(J54:R54)</f>
+        <f t="shared" si="5"/>
         <v>20</v>
       </c>
     </row>
@@ -4218,7 +4234,7 @@
         <v>45610</v>
       </c>
       <c r="C55" s="15" t="s">
-        <v>73</v>
+        <v>100</v>
       </c>
       <c r="D55" s="1">
         <v>9</v>
@@ -4230,11 +4246,11 @@
         <v>11</v>
       </c>
       <c r="G55" s="9">
-        <f>E55/F55</f>
+        <f t="shared" si="3"/>
         <v>198.09090909090909</v>
       </c>
       <c r="H55" s="10">
-        <f>G55/$H$2</f>
+        <f t="shared" si="4"/>
         <v>0.55025252525252522</v>
       </c>
       <c r="I55" s="10"/>
@@ -4266,7 +4282,7 @@
         <v>3</v>
       </c>
       <c r="S55" s="5">
-        <f>SUM(J55:R55)</f>
+        <f t="shared" si="5"/>
         <v>21</v>
       </c>
     </row>
@@ -4278,7 +4294,7 @@
         <v>45497</v>
       </c>
       <c r="C56" s="15" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="D56" s="1">
         <v>9</v>
@@ -4290,11 +4306,11 @@
         <v>11</v>
       </c>
       <c r="G56" s="9">
-        <f>E56/F56</f>
+        <f t="shared" si="3"/>
         <v>254.81818181818181</v>
       </c>
       <c r="H56" s="10">
-        <f>G56/$H$2</f>
+        <f t="shared" si="4"/>
         <v>0.70782828282828281</v>
       </c>
       <c r="I56" s="10"/>
@@ -4326,7 +4342,7 @@
         <v>2</v>
       </c>
       <c r="S56" s="5">
-        <f>SUM(J56:R56)</f>
+        <f t="shared" si="5"/>
         <v>18</v>
       </c>
     </row>
@@ -4338,7 +4354,7 @@
         <v>45497</v>
       </c>
       <c r="C57" s="15" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="D57" s="1">
         <v>9</v>
@@ -4350,11 +4366,11 @@
         <v>11</v>
       </c>
       <c r="G57" s="9">
-        <f>E57/F57</f>
+        <f t="shared" si="3"/>
         <v>1321.2727272727273</v>
       </c>
       <c r="H57" s="10">
-        <f>G57/$H$2</f>
+        <f t="shared" si="4"/>
         <v>3.6702020202020202</v>
       </c>
       <c r="I57" s="10"/>
@@ -4386,7 +4402,7 @@
         <v>3</v>
       </c>
       <c r="S57" s="5">
-        <f>SUM(J57:R57)</f>
+        <f t="shared" si="5"/>
         <v>25</v>
       </c>
     </row>
@@ -4398,7 +4414,7 @@
         <v>45497</v>
       </c>
       <c r="C58" s="15" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="D58" s="1">
         <v>9</v>
@@ -4410,11 +4426,11 @@
         <v>19</v>
       </c>
       <c r="G58" s="9">
-        <f>E58/F58</f>
+        <f t="shared" si="3"/>
         <v>833.47368421052636</v>
       </c>
       <c r="H58" s="10">
-        <f>G58/$H$2</f>
+        <f t="shared" si="4"/>
         <v>2.3152046783625733</v>
       </c>
       <c r="I58" s="10"/>
@@ -4446,7 +4462,7 @@
         <v>3</v>
       </c>
       <c r="S58" s="5">
-        <f>SUM(J58:R58)</f>
+        <f t="shared" si="5"/>
         <v>25</v>
       </c>
     </row>
@@ -4458,7 +4474,7 @@
         <v>45610</v>
       </c>
       <c r="C59" s="15" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="D59" s="1">
         <v>9</v>
@@ -4470,11 +4486,11 @@
         <v>5</v>
       </c>
       <c r="G59" s="9">
-        <f>E59/F59</f>
+        <f t="shared" si="3"/>
         <v>1723.8</v>
       </c>
       <c r="H59" s="10">
-        <f>G59/$H$2</f>
+        <f t="shared" si="4"/>
         <v>4.7883333333333331</v>
       </c>
       <c r="I59" s="10"/>
@@ -4506,7 +4522,7 @@
         <v>3</v>
       </c>
       <c r="S59" s="5">
-        <f>SUM(J59:R59)</f>
+        <f t="shared" si="5"/>
         <v>25</v>
       </c>
     </row>
@@ -4518,7 +4534,7 @@
         <v>45610</v>
       </c>
       <c r="C60" s="15" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="D60" s="1">
         <v>9</v>
@@ -4534,7 +4550,7 @@
         <v>809.15789473684208</v>
       </c>
       <c r="H60" s="10">
-        <f>G60/$H$2</f>
+        <f t="shared" si="4"/>
         <v>2.2476608187134501</v>
       </c>
       <c r="I60" s="10"/>
@@ -4566,7 +4582,7 @@
         <v>3</v>
       </c>
       <c r="S60" s="5">
-        <f>SUM(J60:R60)</f>
+        <f t="shared" si="5"/>
         <v>25</v>
       </c>
     </row>
@@ -4578,7 +4594,7 @@
         <v>45497</v>
       </c>
       <c r="C61" s="15" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
       <c r="D61" s="1">
         <v>9</v>
@@ -4590,11 +4606,11 @@
         <v>11</v>
       </c>
       <c r="G61" s="9">
-        <f>E61/F61</f>
+        <f t="shared" ref="G61:G69" si="6">E61/F61</f>
         <v>1692.8181818181818</v>
       </c>
       <c r="H61" s="10">
-        <f>G61/$H$2</f>
+        <f t="shared" si="4"/>
         <v>4.7022727272727272</v>
       </c>
       <c r="I61" s="10"/>
@@ -4626,7 +4642,7 @@
         <v>3</v>
       </c>
       <c r="S61" s="5">
-        <f>SUM(J61:R61)</f>
+        <f t="shared" si="5"/>
         <v>24</v>
       </c>
     </row>
@@ -4638,7 +4654,7 @@
         <v>45497</v>
       </c>
       <c r="C62" s="15" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="D62" s="1">
         <v>9</v>
@@ -4650,11 +4666,11 @@
         <v>13</v>
       </c>
       <c r="G62" s="9">
-        <f>E62/F62</f>
+        <f t="shared" si="6"/>
         <v>1705.3076923076924</v>
       </c>
       <c r="H62" s="10">
-        <f>G62/$H$2</f>
+        <f t="shared" si="4"/>
         <v>4.7369658119658125</v>
       </c>
       <c r="I62" s="10"/>
@@ -4686,7 +4702,7 @@
         <v>3</v>
       </c>
       <c r="S62" s="5">
-        <f>SUM(J62:R62)</f>
+        <f t="shared" si="5"/>
         <v>24</v>
       </c>
     </row>
@@ -4698,7 +4714,7 @@
         <v>45497</v>
       </c>
       <c r="C63" s="15" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="D63" s="1">
         <v>9</v>
@@ -4710,11 +4726,11 @@
         <v>7</v>
       </c>
       <c r="G63" s="9">
-        <f>E63/F63</f>
+        <f t="shared" si="6"/>
         <v>2243.5714285714284</v>
       </c>
       <c r="H63" s="10">
-        <f>G63/$H$2</f>
+        <f t="shared" si="4"/>
         <v>6.2321428571428568</v>
       </c>
       <c r="I63" s="10"/>
@@ -4746,7 +4762,7 @@
         <v>3</v>
       </c>
       <c r="S63" s="5">
-        <f>SUM(J63:R63)</f>
+        <f t="shared" si="5"/>
         <v>25</v>
       </c>
     </row>
@@ -4758,7 +4774,7 @@
         <v>45497</v>
       </c>
       <c r="C64" s="15" t="s">
-        <v>82</v>
+        <v>101</v>
       </c>
       <c r="D64" s="1">
         <v>9</v>
@@ -4770,11 +4786,11 @@
         <v>19</v>
       </c>
       <c r="G64" s="9">
-        <f>E64/F64</f>
+        <f t="shared" si="6"/>
         <v>223.47368421052633</v>
       </c>
       <c r="H64" s="10">
-        <f>G64/$H$2</f>
+        <f t="shared" si="4"/>
         <v>0.62076023391812873</v>
       </c>
       <c r="I64" s="10"/>
@@ -4806,7 +4822,7 @@
         <v>3</v>
       </c>
       <c r="S64" s="5">
-        <f>SUM(J64:R64)</f>
+        <f t="shared" si="5"/>
         <v>21</v>
       </c>
     </row>
@@ -4818,7 +4834,7 @@
         <v>45497</v>
       </c>
       <c r="C65" s="16" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="D65" s="1">
         <v>9</v>
@@ -4830,11 +4846,11 @@
         <v>11</v>
       </c>
       <c r="G65" s="9">
-        <f>E65/F65</f>
+        <f t="shared" si="6"/>
         <v>415.72727272727275</v>
       </c>
       <c r="H65" s="10">
-        <f>G65/$H$2</f>
+        <f t="shared" si="4"/>
         <v>1.1547979797979799</v>
       </c>
       <c r="I65" s="10"/>
@@ -4866,7 +4882,7 @@
         <v>3</v>
       </c>
       <c r="S65" s="5">
-        <f>SUM(J65:R65)</f>
+        <f t="shared" si="5"/>
         <v>21</v>
       </c>
     </row>
@@ -4878,7 +4894,7 @@
         <v>45610</v>
       </c>
       <c r="C66" s="15" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="D66" s="1">
         <v>9</v>
@@ -4890,11 +4906,11 @@
         <v>11</v>
       </c>
       <c r="G66" s="9">
-        <f>E66/F66</f>
+        <f t="shared" si="6"/>
         <v>479.90909090909093</v>
       </c>
       <c r="H66" s="10">
-        <f>G66/$H$2</f>
+        <f t="shared" si="4"/>
         <v>1.3330808080808081</v>
       </c>
       <c r="I66" s="10"/>
@@ -4926,7 +4942,7 @@
         <v>3</v>
       </c>
       <c r="S66" s="5">
-        <f>SUM(J66:R66)</f>
+        <f t="shared" si="5"/>
         <v>22</v>
       </c>
     </row>
@@ -4938,7 +4954,7 @@
         <v>45498</v>
       </c>
       <c r="C67" s="15" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="D67" s="1">
         <v>9</v>
@@ -4950,11 +4966,11 @@
         <v>15</v>
       </c>
       <c r="G67" s="9">
-        <f>E67/F67</f>
+        <f t="shared" si="6"/>
         <v>236.6</v>
       </c>
       <c r="H67" s="10">
-        <f>G67/$H$2</f>
+        <f t="shared" si="4"/>
         <v>0.65722222222222215</v>
       </c>
       <c r="I67" s="10"/>
@@ -4986,7 +5002,7 @@
         <v>3</v>
       </c>
       <c r="S67" s="5">
-        <f>SUM(J67:R67)</f>
+        <f t="shared" si="5"/>
         <v>21</v>
       </c>
     </row>
@@ -4998,7 +5014,7 @@
         <v>45497</v>
       </c>
       <c r="C68" s="15" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="D68" s="1">
         <v>9</v>
@@ -5010,11 +5026,11 @@
         <v>15</v>
       </c>
       <c r="G68" s="9">
-        <f>E68/F68</f>
+        <f t="shared" si="6"/>
         <v>299.2</v>
       </c>
       <c r="H68" s="10">
-        <f>G68/$H$2</f>
+        <f t="shared" ref="H68:H99" si="7">G68/$H$2</f>
         <v>0.83111111111111113</v>
       </c>
       <c r="I68" s="10"/>
@@ -5046,7 +5062,7 @@
         <v>3</v>
       </c>
       <c r="S68" s="5">
-        <f>SUM(J68:R68)</f>
+        <f t="shared" ref="S68:S99" si="8">SUM(J68:R68)</f>
         <v>22</v>
       </c>
     </row>
@@ -5058,7 +5074,7 @@
         <v>45497</v>
       </c>
       <c r="C69" s="15" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="D69" s="1">
         <v>9</v>
@@ -5070,11 +5086,11 @@
         <v>15</v>
       </c>
       <c r="G69" s="9">
-        <f>E69/F69</f>
+        <f t="shared" si="6"/>
         <v>171.13333333333333</v>
       </c>
       <c r="H69" s="10">
-        <f>G69/$H$2</f>
+        <f t="shared" si="7"/>
         <v>0.47537037037037033</v>
       </c>
       <c r="I69" s="10"/>
@@ -5106,11 +5122,11 @@
         <v>3</v>
       </c>
       <c r="S69" s="5">
-        <f>SUM(J69:R69)</f>
+        <f t="shared" si="8"/>
         <v>21</v>
       </c>
     </row>
-    <row r="70" spans="1:19" ht="15.75">
+    <row r="70" spans="1:19" ht="15.6">
       <c r="A70" s="14">
         <v>92</v>
       </c>
@@ -5118,7 +5134,7 @@
         <v>46012</v>
       </c>
       <c r="C70" s="15" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="D70" s="1">
         <v>9</v>
@@ -5134,7 +5150,7 @@
         <v>530.90909090909088</v>
       </c>
       <c r="H70" s="10">
-        <f>G70/$H$2</f>
+        <f t="shared" si="7"/>
         <v>1.4747474747474747</v>
       </c>
       <c r="I70" s="43" t="s">
@@ -5168,7 +5184,7 @@
         <v>3</v>
       </c>
       <c r="S70" s="5">
-        <f>SUM(J70:R70)</f>
+        <f t="shared" si="8"/>
         <v>22</v>
       </c>
     </row>
@@ -5180,7 +5196,7 @@
         <v>45610</v>
       </c>
       <c r="C71" s="15" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="D71" s="1">
         <v>9</v>
@@ -5196,7 +5212,7 @@
         <v>198.42857142857142</v>
       </c>
       <c r="H71" s="10">
-        <f>G71/$H$2</f>
+        <f t="shared" si="7"/>
         <v>0.55119047619047612</v>
       </c>
       <c r="I71" s="10"/>
@@ -5228,7 +5244,7 @@
         <v>3</v>
       </c>
       <c r="S71" s="5">
-        <f>SUM(J71:R71)</f>
+        <f t="shared" si="8"/>
         <v>21</v>
       </c>
     </row>
@@ -5240,7 +5256,7 @@
         <v>45497</v>
       </c>
       <c r="C72" s="15" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="D72" s="1">
         <v>9</v>
@@ -5256,7 +5272,7 @@
         <v>100.2</v>
       </c>
       <c r="H72" s="10">
-        <f>G72/$H$2</f>
+        <f t="shared" si="7"/>
         <v>0.27833333333333332</v>
       </c>
       <c r="I72" s="10"/>
@@ -5288,7 +5304,7 @@
         <v>3</v>
       </c>
       <c r="S72" s="5">
-        <f>SUM(J72:R72)</f>
+        <f t="shared" si="8"/>
         <v>19</v>
       </c>
     </row>
@@ -5300,7 +5316,7 @@
         <v>45610</v>
       </c>
       <c r="C73" s="15" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="D73" s="1">
         <v>9</v>
@@ -5316,7 +5332,7 @@
         <v>175.18181818181819</v>
       </c>
       <c r="H73" s="10">
-        <f>G73/$H$2</f>
+        <f t="shared" si="7"/>
         <v>0.48661616161616161</v>
       </c>
       <c r="I73" s="10"/>
@@ -5348,7 +5364,7 @@
         <v>3</v>
       </c>
       <c r="S73" s="5">
-        <f>SUM(J73:R73)</f>
+        <f t="shared" si="8"/>
         <v>21</v>
       </c>
     </row>
@@ -5360,7 +5376,7 @@
         <v>45497</v>
       </c>
       <c r="C74" s="15" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="D74" s="1">
         <v>9</v>
@@ -5376,7 +5392,7 @@
         <v>215.18181818181819</v>
       </c>
       <c r="H74" s="10">
-        <f>G74/$H$2</f>
+        <f t="shared" si="7"/>
         <v>0.59772727272727277</v>
       </c>
       <c r="I74" s="10"/>
@@ -5408,7 +5424,7 @@
         <v>3</v>
       </c>
       <c r="S74" s="5">
-        <f>SUM(J74:R74)</f>
+        <f t="shared" si="8"/>
         <v>20</v>
       </c>
     </row>
@@ -5420,7 +5436,7 @@
         <v>45610</v>
       </c>
       <c r="C75" s="15" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="D75" s="1">
         <v>8</v>
@@ -5436,7 +5452,7 @@
         <v>211.06666666666666</v>
       </c>
       <c r="H75" s="10">
-        <f>G75/$H$2</f>
+        <f t="shared" si="7"/>
         <v>0.58629629629629632</v>
       </c>
       <c r="I75" s="10"/>
@@ -5468,18 +5484,18 @@
         <v>3</v>
       </c>
       <c r="S75" s="5">
-        <f>SUM(J75:R75)</f>
+        <f t="shared" si="8"/>
         <v>20</v>
       </c>
     </row>
     <row r="76" spans="1:19" ht="26.25" customHeight="1">
       <c r="F76" s="21" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
     </row>
     <row r="77" spans="1:19" ht="54.75" customHeight="1">
       <c r="C77" s="17" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
     </row>
     <row r="78" spans="1:19">
@@ -5490,7 +5506,7 @@
         <v>45747</v>
       </c>
       <c r="C78" s="16" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
       <c r="D78" s="1">
         <v>3</v>
@@ -5527,7 +5543,7 @@
       <c r="R78" s="22"/>
       <c r="S78" s="25"/>
     </row>
-    <row r="79" spans="1:19" ht="15.75">
+    <row r="79" spans="1:19" ht="15.6">
       <c r="A79" s="14">
         <v>50</v>
       </c>
@@ -5535,7 +5551,7 @@
         <v>45916</v>
       </c>
       <c r="C79" s="16" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="D79" s="1">
         <v>9</v>
@@ -5547,7 +5563,7 @@
         <v>11</v>
       </c>
       <c r="G79" s="9">
-        <f t="shared" ref="G79:G84" si="0">E79/F79</f>
+        <f t="shared" ref="G79:G84" si="9">E79/F79</f>
         <v>1.3636363636363635</v>
       </c>
       <c r="H79" s="10">
@@ -5572,7 +5588,7 @@
       <c r="R79" s="31"/>
       <c r="S79" s="33"/>
     </row>
-    <row r="80" spans="1:19" ht="15.75">
+    <row r="80" spans="1:19" ht="15.6">
       <c r="A80" s="14">
         <v>94</v>
       </c>
@@ -5580,7 +5596,7 @@
         <v>46028</v>
       </c>
       <c r="C80" s="16" t="s">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="D80" s="1"/>
       <c r="E80" s="41"/>
@@ -5588,11 +5604,11 @@
         <v>11</v>
       </c>
       <c r="G80" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="H80" s="44">
-        <f t="shared" ref="H79:H84" si="1">G80/$H$2</f>
+        <f t="shared" ref="H80:H84" si="10">G80/$H$2</f>
         <v>0</v>
       </c>
       <c r="I80" s="43" t="s">
@@ -5613,7 +5629,7 @@
       <c r="R80" s="5"/>
       <c r="S80" s="5"/>
     </row>
-    <row r="81" spans="1:19" ht="15.75">
+    <row r="81" spans="1:19" ht="15.6">
       <c r="A81" s="14">
         <v>91</v>
       </c>
@@ -5621,7 +5637,7 @@
         <v>45973</v>
       </c>
       <c r="C81" s="16" t="s">
-        <v>99</v>
+        <v>84</v>
       </c>
       <c r="D81" s="1">
         <v>3</v>
@@ -5631,11 +5647,11 @@
         <v>15</v>
       </c>
       <c r="G81" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="H81" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="I81" s="43" t="s">
@@ -5656,7 +5672,7 @@
       <c r="R81" s="35"/>
       <c r="S81" s="37"/>
     </row>
-    <row r="82" spans="1:19" ht="15.75">
+    <row r="82" spans="1:19" ht="15.6">
       <c r="A82" s="14">
         <v>90</v>
       </c>
@@ -5664,7 +5680,7 @@
         <v>45973</v>
       </c>
       <c r="C82" s="16" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
       <c r="D82" s="1">
         <v>9</v>
@@ -5674,11 +5690,11 @@
         <v>17</v>
       </c>
       <c r="G82" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="H82" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="I82" s="43" t="s">
@@ -5707,7 +5723,7 @@
         <v>45841</v>
       </c>
       <c r="C83" s="16" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D83" s="1"/>
       <c r="E83" s="5">
@@ -5717,7 +5733,7 @@
         <v>11</v>
       </c>
       <c r="G83" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>44.545454545454547</v>
       </c>
       <c r="H83" s="10">
@@ -5748,7 +5764,7 @@
         <v>46022</v>
       </c>
       <c r="C84" s="16" t="s">
-        <v>102</v>
+        <v>86</v>
       </c>
       <c r="D84" s="1">
         <v>1</v>
@@ -5758,11 +5774,11 @@
         <v>11</v>
       </c>
       <c r="G84" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="H84" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="I84" s="10"/>
@@ -5789,7 +5805,7 @@
     </row>
     <row r="86" spans="1:19" ht="54" customHeight="1">
       <c r="C86" s="29" t="s">
-        <v>103</v>
+        <v>87</v>
       </c>
       <c r="D86" s="38">
         <v>7.0000000000000007E-2</v>
@@ -5805,7 +5821,10 @@
   <mergeCells count="1">
     <mergeCell ref="K2:S2"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="C54" r:id="rId1" xr:uid="{FCE3B167-AC64-4448-9E61-D08165831574}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>